<commit_message>
First commit for IPSL atmosphere realm spreadsheet (not complete yet).
</commit_message>
<xml_diff>
--- a/cmip6/citations/cmip6_ipsl_citations.xlsx
+++ b/cmip6/citations/cmip6_ipsl_citations.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="221">
   <si>
     <t>ES-DOC CMIP6 Model Citations</t>
   </si>
@@ -527,12 +527,559 @@
   <si>
     <t>https://www.geosci-model-dev.net/9/363/2016/gmd-9-363-2016.html</t>
   </si>
+  <si>
+    <t>Sadourny1984</t>
+  </si>
+  <si>
+    <t>"@incollection{
+   author = {Sadourny,R. and Laval,K.},
+   address = {Amsterdam},
+   booktitle = {New perspectives in Climate Modeling},
+   editor = {A.~Berger and C.~Nicolis},
+   key = {Sadourny, Laval, 1984},
+   pages = {173-197},
+   series = {Elsevier},
+   title = {January and {July} performance of the \protect{LMD} General Circulation Model},
+   year = {1984}
+}"</t>
+  </si>
+  <si>
+    <t>New perspectives in Climate Modeling</t>
+  </si>
+  <si>
+    <t>VanLeer1977</t>
+  </si>
+  <si>
+    <t>Towards the ultimate conservative difference scheme : {IV.} A new approach to numerical convection</t>
+  </si>
+  <si>
+    <t>"@article{
+   author = {Van Leer , Bram},
+   journal = {J. Computational Phys.},
+   pages = {276-299},
+   title = {Towards the ultimate conservative difference scheme : {IV.} A new approach to numerical convection},
+   volume = {23},
+   year = {1977}
+}"</t>
+  </si>
+  <si>
+    <t>Hourdin1999</t>
+  </si>
+  <si>
+    <t>"@article{
+   author = {Hourdin , F. and Armengaud , A.},
+   journal = {Mon. Wea. Rev.},
+   pages = {822--837},
+   title = {The Use of Finite-Volume Methods for Atmospheric Advection of Trace Species. Part I: Test of Vairious Formulations in a General Circulation Model},
+   volume = {127},
+   year = {1999}
+}"</t>
+  </si>
+  <si>
+    <t>The Use of Finite-Volume Methods for Atmospheric Advection of Trace Species. Part I: Test of Vairious Formulations in a General Circulation Model</t>
+  </si>
+  <si>
+    <t>LMDZ5B: the atmospheric component of the IPSL climate model with revisited parameterizations for clouds and convection</t>
+  </si>
+  <si>
+    <t>Hourdin2013a</t>
+  </si>
+  <si>
+    <t>10.1007/s00382-012-1343-y</t>
+  </si>
+  <si>
+    <t>http://adsabs.harvard.edu/abs/2013ClDy...40.2193H</t>
+  </si>
+  <si>
+    <t>"@article{
+   author = {{Hourdin}, F. and {Grandpeix}, J.-Y. and {Rio}, C. and {Bony}, S. and {Jam}, A. and {Cheruy}, F. and {Rochetin}, N. and {Fairhead}, L. and {Idelkadi}, A. and {Musat}, I. and {Dufresne}, J.-L. and {Lahellec}, A. and {Lefebvre}, M.-P. and {Roehrig}, R.},
+    title = "{LMDZ5B: the atmospheric component of the IPSL climate model with revisited parameterizations for clouds and convection}",
+  journal = {Clim. Dyn},
+ keywords = {Climate modeling, Physical parameterizations, Shallow convection, Deep convection, Climate change projections},
+     year = 2013,
+    month = may,
+   volume = 40,
+    pages = {2193-2222},
+      doi = {10.1007/s00382-012-1343-y},
+   adsurl = {http://adsabs.harvard.edu/abs/2013ClDy...40.2193H},
+  adsnote = {Provided by the SAO/NASA Astrophysics Data System}
+}"</t>
+  </si>
+  <si>
+    <t>Hourdin2013b</t>
+  </si>
+  <si>
+    <t>10.1007/s00382-012-1411-3</t>
+  </si>
+  <si>
+    <t>http://adsabs.harvard.edu/abs/2013ClDy...40.2167H</t>
+  </si>
+  <si>
+    <t>Impact of the LMDZ atmospheric grid configuration on the climate and sensitivity of the IPSL-CM5A coupled model</t>
+  </si>
+  <si>
+    <t>"@article{
+   author = {{Hourdin}, F. and {Foujols}, M.-A. and {Codron}, F. and {Guemas}, V. and {Dufresne}, J.-L. and {Bony}, S. and {Denvil}, S. and {Guez}, L. and {Lott}, F. and {Ghattas}, J. and {Braconnot}, P. and {Marti}, O. and {Meurdesoif}, Y. and {Bopp}, L.},
+    title = "{Impact of the LMDZ atmospheric grid configuration on the climate and sensitivity of the IPSL-CM5A coupled model}",
+  journal = {Clim. Dyn.},
+ keywords = {Climate modeling, Grid resolution, Climate change projections},
+     year = 2013,
+    month = may,
+   volume = 40,
+    pages = {2167-2192},
+      doi = {10.1007/s00382-012-1411-3},
+   adsurl = {http://adsabs.harvard.edu/abs/2013ClDy...40.2167H},
+  adsnote = {Provided by the SAO/NASA Astrophysics Data System}
+}"</t>
+  </si>
+  <si>
+    <t>Yamada1983</t>
+  </si>
+  <si>
+    <t>"@article{
+   author = {Yamada , T.},
+   journal = {J. Atmos. Sci.},
+   pages = {91--106},
+   title = {Simulations of Nocturnal Drainage Flows by a $q^2l$ Turbulence Closure Model},
+   volume = {40},
+   year = {1983}
+}"</t>
+  </si>
+  <si>
+    <t>Hourdin2002</t>
+  </si>
+  <si>
+    <t>"@article{
+   author = {Hourdin , F. and Couvreux , F. and Menut , L.},
+   journal = {J. Atmos. Sci.},
+   title = {Parameterisation of the dry convective boundary layer based on a mass flux representation of thermals},
+   volume = {59},
+   pages = {1105--1123},
+   year = {2002}
+}"</t>
+  </si>
+  <si>
+    <t>Parameterisation of the dry convective boundary layer based on a mass flux representation of thermals</t>
+  </si>
+  <si>
+    <t>Simulations of Nocturnal Drainage Flows by a q²l Turbulence Closure Model</t>
+  </si>
+  <si>
+    <t>Rio2008</t>
+  </si>
+  <si>
+    <t>"@article{Rio:08,
+   author = {Rio , C. and Hourdin , F.},
+   title={A thermal plume model for the convective boundary layer : Representation of cumulus clouds},
+   journal={J. Atmos. Sci.},
+   volume=65,
+   pages={407--425},
+   year = {2008}
+}"</t>
+  </si>
+  <si>
+    <t>A thermal plume model for the convective boundary layer : Representation of cumulus clouds</t>
+  </si>
+  <si>
+    <t>10.1029/2008GL036779</t>
+  </si>
+  <si>
+    <t>http://adsabs.harvard.edu/abs/2009GeoRL..3607809R</t>
+  </si>
+  <si>
+    <t>"@article{
+   author = {{Rio}, C. and {Hourdin}, F. and {Grandpeix}, {J.-Y.} and {Lafore}, {J.-P.}
+        },
+    title = "{Shifting the diurnal cycle of parameterized deep convection over land}",
+  journal = grl,
+ keywords = {Atmospheric Processes: Convective processes, Atmospheric Processes: Boundary layer processes, Atmospheric Processes: Precipitation (1854), Atmospheric Processes: Global climate models (1626, 4928)},
+     year = 2009,
+    month = apr,
+   volume = 36,
+    pages = {7809-+},
+      doi = {10.1029/2008GL036779},
+   adsurl = {http://adsabs.harvard.edu/abs/2009GeoRL..3607809R},
+  adsnote = {Provided by the SAO/NASA Astrophysics Data System}
+}"</t>
+  </si>
+  <si>
+    <t>Shifting the diurnal cycle of parameterized deep convection over land</t>
+  </si>
+  <si>
+    <t>Rio2009</t>
+  </si>
+  <si>
+    <t>Rio2010</t>
+  </si>
+  <si>
+    <t>10.1007/s10546-010-9478-z</t>
+  </si>
+  <si>
+    <t>http://adsabs.harvard.edu/abs/2010BoLMe.135..469R</t>
+  </si>
+  <si>
+    <t>Boundary-layer thermals, Entrainment and detrainment, Large-eddy simulations, Mass-flux parametrization</t>
+  </si>
+  <si>
+    <t>"@article{
+   author = {{Rio}, C. and {Hourdin}, F. and {Couvreux}, F. and {Jam}, A.},
+    title = "{Resolved Versus Parametrized Boundary-Layer Plumes. Part II: Continuous Formulations of Mixing Rates for Mass-Flux Schemes}",
+  journal = blm,
+ keywords = {Boundary-layer thermals, Entrainment and detrainment, Large-eddy simulations, Mass-flux parametrization},
+     year = 2010,
+    month = jun,
+   volume = 135,
+    pages = {469-483},
+      doi = {10.1007/s10546-010-9478-z},
+   adsurl = {http://adsabs.harvard.edu/abs/2010BoLMe.135..469R},
+  adsnote = {Provided by the SAO/NASA Astrophysics Data System}
+}"</t>
+  </si>
+  <si>
+    <t>10.1175/2009JAS3045.1</t>
+  </si>
+  <si>
+    <t>http://adsabs.harvard.edu/abs/2010JAtS...67..898G</t>
+  </si>
+  <si>
+    <t>A Density Current Parameterization Coupled with Emanuel's Convection Scheme. Part II: 1D Simulations</t>
+  </si>
+  <si>
+    <t>"@article{
+   author = {{Grandpeix}, {J.-Y.} and {Lafore}, {J.-P.} and {Cheruy}, F.},
+    title = "{A Density Current Parameterization Coupled with Emanuel's Convection Scheme. Part II: 1D Simulations}",
+  journal = {Journal of Atmospheric Sciences},
+     year = 2010,
+    month = apr,
+   volume = 67,
+    pages = {898-922},
+      doi = {10.1175/2009JAS3045.1},
+   adsurl = {http://adsabs.harvard.edu/abs/2010JAtS...67..898G},
+  adsnote = {Provided by the SAO/NASA Astrophysics Data System}
+}"</t>
+  </si>
+  <si>
+    <t>Grandpeix2010b</t>
+  </si>
+  <si>
+    <t>Grandpeix2010a</t>
+  </si>
+  <si>
+    <t>"@article{
+   author = {{Grandpeix}, {J.-Y.} and {Lafore}, {J.-P.}},
+    title = "{A Density Current Parameterization Coupled with Emanuel's Convection Scheme. Part I: The Models}",
+  journal = {Journal of Atmospheric Sciences},
+     year = 2010,
+    month = apr,
+   volume = 67,
+    pages = {881-897},
+      doi = {10.1175/2009JAS3044.1},
+   adsurl = {http://adsabs.harvard.edu/abs/2010JAtS...67..881G},
+  adsnote = {Provided by the SAO/NASA Astrophysics Data System}
+}"</t>
+  </si>
+  <si>
+    <t>10.1175/2009JAS3044.1</t>
+  </si>
+  <si>
+    <t>http://adsabs.harvard.edu/abs/2010JAtS...67..881G</t>
+  </si>
+  <si>
+    <t>A Density Current Parameterization Coupled with Emanuel's Convection Scheme. Part I: The Models</t>
+  </si>
+  <si>
+    <t>Bony2001</t>
+  </si>
+  <si>
+    <t>A parameterization of the Cloudiness Associated with Cumulus Convection; Evaluation Using TOGA COARE Data</t>
+  </si>
+  <si>
+    <t>"@article{
+   author  = {Bony , S. and Emanuel , K. A.},
+   title = {A parameterization of the Cloudiness Associated with Cumulus Convection; Evaluation Using {TOGA COARE} Data},
+   journal = {J. Atmos. Sci.},
+   volume = 58,
+   pages = {3158--3183},
+   year = 2001
+}"</t>
+  </si>
+  <si>
+    <t>Jam2013</t>
+  </si>
+  <si>
+    <t>Resolved Versus Parametrized Boundary-Layer Plumes. Part III: Derivation of a Statistical Scheme for Cumulus Clouds</t>
+  </si>
+  <si>
+    <t>http://adsabs.harvard.edu/abs/2013BoLMe.147..421J</t>
+  </si>
+  <si>
+    <t>10.1007/s10546-012-9789-3</t>
+  </si>
+  <si>
+    <t>"@article{
+   author = {{Jam}, A. and {Hourdin}, F. and {Rio}, C. and {Couvreux}, F.  },
+    title = "{Resolved Versus Parametrized Boundary-Layer Plumes. Part III: Derivation of a Statistical Scheme for Cumulus Clouds}",
+  journal = {Boundary-layer Meteorol.},
+ keywords = {Boundary-layer thermals, Cloud scheme, Conditional sampling, Large-eddy simulations, Probability distribution function},
+     year = 2013,
+    month = jun,
+   volume = 147,
+    pages = {421-441},
+      doi = {10.1007/s10546-012-9789-3},
+   adsurl = {http://adsabs.harvard.edu/abs/2013BoLMe.147..421J},
+  adsnote = {Provided by the SAO/NASA Astrophysics Data System}
+}"</t>
+  </si>
+  <si>
+    <t>Rochetin2014a</t>
+  </si>
+  <si>
+    <t>10.1175/JAS-D-12-0336.1</t>
+  </si>
+  <si>
+    <t>https://ui.adsabs.harvard.edu/#abs/2014JAtS...71..496R</t>
+  </si>
+  <si>
+    <t>Deep Convection Triggering by Boundary Layer Thermals. Part I: LES Analysis and Stochastic Triggering Formulation</t>
+  </si>
+  <si>
+    <t>"@article{
+       author = {{Rochetin}, Nicolas and {Couvreux}, Fleur and {Grandpeix}, Jean-Yves and {Rio}, Catherine},
+        title = "{Deep Convection Triggering by Boundary Layer Thermals. Part I: LES Analysis and Stochastic Triggering Formulation}",
+      journal = jas,
+         year = 2014,
+        month = Feb,
+       volume = {71},
+        pages = {496-514},
+          doi = {10.1175/JAS-D-12-0336.1},
+       adsurl = {https://ui.adsabs.harvard.edu/#abs/2014JAtS...71..496R},
+      adsnote = {Provided by the SAO/NASA Astrophysics Data System}
+}"</t>
+  </si>
+  <si>
+    <t>Rochetin2014b</t>
+  </si>
+  <si>
+    <t>"@article{
+       author = {{Rochetin}, Nicolas and {Grandpeix}, Jean-Yves and {Rio}, Catherine and {Couvreux}, Fleur},
+        title = "{Deep Convection Triggering by Boundary Layer Thermals. Part II: Stochastic Triggering Parameterization for the LMDZ GCM}",
+      journal = {J. Atmos. Sci.},
+         year = 2014,
+        month = Feb,
+       volume = {71},
+        pages = {515-538},
+          doi = {10.1175/JAS-D-12-0337.1},
+       adsurl = {https://ui.adsabs.harvard.edu/#abs/2014JAtS...71..515R},
+      adsnote = {Provided by the SAO/NASA Astrophysics Data System}
+}"</t>
+  </si>
+  <si>
+    <t>10.1175/JAS-D-12-0337.1</t>
+  </si>
+  <si>
+    <t>https://ui.adsabs.harvard.edu/#abs/2014JAtS...71..515R</t>
+  </si>
+  <si>
+    <t>Deep Convection Triggering by Boundary Layer Thermals. Part II: Stochastic Triggering Parameterization for the LMDZ GCM</t>
+  </si>
+  <si>
+    <t>Lott2013</t>
+  </si>
+  <si>
+    <t>10.1002/jgrd.50705</t>
+  </si>
+  <si>
+    <t>A Stochastic Parameterization of the Gravity Waves Due to Convection and Its Impact on the Equatorial Stratosphere</t>
+  </si>
+  <si>
+    <t>"@article{
+    author      = {Lott, F. and Guez, L.},
+    year        = 2013,
+    title       = {A Stochastic Parameterization of the Gravity Waves Due to Convection and Its Impact on the Equatorial Stratosphere},
+    journal     = {J. Geophys. Res.},
+    volume      = 118,
+    pages       = {8897--8909},
+    doi         = {10.1002/jgrd.50705}
+}"</t>
+  </si>
+  <si>
+    <t>delaCamara2015</t>
+  </si>
+  <si>
+    <t>10.1002/GL063298</t>
+  </si>
+  <si>
+    <t>"@article{
+    author      = {de~la C\'{a}mara, A. and Lott, F.},
+    year        = 2015,
+    title       = {A Stochastic Parameterization of the Gravity Waves Emitted by Fronts and Jets},
+    journal     = {Geophys. Res. Lett.},
+    volume      = 42,
+    pages       = {2071--2078},
+    doi         = {10.1002/GL063298}
+}"</t>
+  </si>
+  <si>
+    <t>A Stochastic Parameterization of the Gravity Waves Emitted by Fronts and Jets</t>
+  </si>
+  <si>
+    <t>Lott2015</t>
+  </si>
+  <si>
+    <t>10.1007/s00382-005-0064-x</t>
+  </si>
+  <si>
+    <t>The stratospheric version of LMDz: Dynamical Climatologies, Arctic Oscillation, and Impact on the Surface Climate</t>
+  </si>
+  <si>
+    <t>"@article{
+    author      = {Lott, F. and Fairhead, L. and Hourdin, F. and Levan, P.},
+    year        = 2005,
+    title       = {The stratospheric version of LMDz: Dynamical Climatologies, Arctic Oscillation, and Impact on the Surface Climate},
+    journal     = {Clim. Dyn.},
+    volume      = 25,
+    pages       = {851--868},
+    doi         = {10.1007/s00382-005-0064-x}
+}"</t>
+  </si>
+  <si>
+    <t>Hines1997</t>
+  </si>
+  <si>
+    <t>"@article{
+author = {Hines, C.~O.},
+number = {4},
+pages = {387--400},
+title = {{Doppler-spread parameterization of gravity-wave momentum deposition in the middle atmosphere. Part 2: Broad and quasi monochromatic spectra, and implementation}},
+journal = {J. of Atmosph. and Solar-Terrestrial Phys.},
+volume = {59},
+year = {1997}
+}"</t>
+  </si>
+  <si>
+    <t>Doppler-spread parameterization of gravity-wave momentum deposition in the middle atmosphere. Part 2: Broad and quasi monochromatic spectra, and implementation</t>
+  </si>
+  <si>
+    <t>"@article{
+author = {de la C\'{a}mara, A. and Lott, F. and Abalos, M.},
+title = {Climatology of the middle atmosphere in LMDz: Impact of source-related parameterizations of gravity wave drag},
+journal = {J. of Adv. in Modeling Earth Systems},
+volume = {8},
+number = {4},
+pages = {1507-1525},
+year = {2016}
+}"</t>
+  </si>
+  <si>
+    <t>delaCamara2016</t>
+  </si>
+  <si>
+    <t>Climatology of the middle atmosphere in LMDz: Impact of source-related parameterizations of gravity wave drag</t>
+  </si>
+  <si>
+    <t>Fouquart1980</t>
+  </si>
+  <si>
+    <t>Computations of solar heating of the Earth’s atmosphere: a new parametrization</t>
+  </si>
+  <si>
+    <t>"@article{
+author={Mlawer, E.J. and S.J. Taubman and P.D. Brown and M.J. Iacono and S.A. Clough},
+year=1997,
+title={Radiative transfer for inhomogeneous atmospheres: {RRTM}, a validated correlated-k model for the longwave},
+journal={J. Geophys. Res.},
+volume={102D},
+pages={16663--16,682}
+}"</t>
+  </si>
+  <si>
+    <t>Mlawer1997</t>
+  </si>
+  <si>
+    <t>Radiative transfer for inhomogeneous atmospheres: RRTM, a validated correlated-k model for the longwave</t>
+  </si>
+  <si>
+    <t>LeTreut1991</t>
+  </si>
+  <si>
+    <t>Sensitivity of an atmospheric general circulation model to prescribed SST changes: Feedback effects associated with the simulation of cloud optical properties</t>
+  </si>
+  <si>
+    <t>"@article{
+  title={Sensitivity of an atmospheric general circulation model to prescribed {SST} changes: Feedback effects associated with the simulation of cloud optical properties},
+  author={Le Treut, Herv{\'e} and Li, Zhao-Xin},
+  journal={Climate Dynamics},
+  volume={5},
+  number={3},
+  pages={175--187},
+  year={1991},
+  publisher={Springer}
+}"</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/profile/Bram_Van_Leer/publication/266987705_Towards_the_Ultimate_Conservative_Difference_Scheme_IV_A_New_Approach_to_Numerical_Convection/links/59ea1757aca272cddddb73e8/Towards-the-Ultimate-Conservative-Difference-Scheme-IV-A-New-Approach-to-Numerical-Convection.pdf</t>
+  </si>
+  <si>
+    <t>https://journals.ametsoc.org/doi/pdf/10.1175/1520-0493(1999)127%3C0822%3ATUOFVM%3E2.0.CO%3B2</t>
+  </si>
+  <si>
+    <t>https://journals.ametsoc.org/doi/pdf/10.1175/1520-0469(1983)040%3C0091:SONDFB%3E2.0.CO;2</t>
+  </si>
+  <si>
+    <t>https://journals.ametsoc.org/doi/pdf/10.1175/1520-0469(2002)059%3C1105%3APOTDCB%3E2.0.CO%3B2</t>
+  </si>
+  <si>
+    <t>https://journals.ametsoc.org/doi/pdf/10.1175/1520-0469(2001)058%3C3158%3AAPOTCA%3E2.0.CO%3B2</t>
+  </si>
+  <si>
+    <t>https://agupubs.onlinelibrary.wiley.com/doi/pdf/10.1002/jgrd.50705</t>
+  </si>
+  <si>
+    <t>https://agupubs.onlinelibrary.wiley.com/doi/pdf/10.1002/2015GL063298</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007/s00382-005-0064-x</t>
+  </si>
+  <si>
+    <t>10.1016/S1364-6826(96)00080-6</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S1364682696000806</t>
+  </si>
+  <si>
+    <t>https://agupubs.onlinelibrary.wiley.com/doi/pdf/10.1002/2016MS000753</t>
+  </si>
+  <si>
+    <t>10.1002/2016MS000753</t>
+  </si>
+  <si>
+    <t>"@article{
+author={Fouquart Y and Bonnel B},
+year=1980,
+title={Computations of solar heating of the Earth’s atmosphere: a new parametrization},
+journal={Contrib. Atmos. Phys.},
+volume=53,
+pages={35--62}
+}"</t>
+  </si>
+  <si>
+    <t>https://agupubs.onlinelibrary.wiley.com/doi/abs/10.1029/97JD00237</t>
+  </si>
+  <si>
+    <t>10.1029/97JD00237</t>
+  </si>
+  <si>
+    <t>10.1007/BF00251808</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/content/pdf/10.1007/BF00251808.pdf</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -599,6 +1146,12 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Helvetica Neue"/>
     </font>
   </fonts>
   <fills count="7">
@@ -752,12 +1305,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -879,8 +1435,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2809,10 +3369,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IP52"/>
+  <dimension ref="A1:IP53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -8091,173 +8651,391 @@
       <c r="IO22" s="39"/>
       <c r="IP22" s="39"/>
     </row>
-    <row r="23" spans="1:250" ht="20.100000000000001" customHeight="1">
-      <c r="A23" s="17"/>
+    <row r="23" spans="1:250" ht="144.75" customHeight="1">
+      <c r="A23" s="17" t="s">
+        <v>112</v>
+      </c>
       <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
+      <c r="C23" s="14" t="s">
+        <v>113</v>
+      </c>
       <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-    </row>
-    <row r="24" spans="1:250" ht="20.100000000000001" customHeight="1">
-      <c r="A24" s="17"/>
+      <c r="E23" s="14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:250" ht="118.5" customHeight="1">
+      <c r="A24" s="17" t="s">
+        <v>115</v>
+      </c>
       <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-    </row>
-    <row r="25" spans="1:250" ht="20.100000000000001" customHeight="1">
-      <c r="A25" s="17"/>
+      <c r="C24" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:250" ht="117.75" customHeight="1">
+      <c r="A25" s="17" t="s">
+        <v>118</v>
+      </c>
       <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-    </row>
-    <row r="26" spans="1:250" ht="20.100000000000001" customHeight="1">
-      <c r="A26" s="17"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-    </row>
-    <row r="27" spans="1:250" ht="20.100000000000001" customHeight="1">
-      <c r="A27" s="17"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-    </row>
-    <row r="28" spans="1:250" ht="20.100000000000001" customHeight="1">
-      <c r="A28" s="17"/>
+      <c r="C25" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:250" ht="217.5" customHeight="1">
+      <c r="A26" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="1:250" ht="209.25" customHeight="1">
+      <c r="A27" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="D27" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:250" ht="107.25" customHeight="1">
+      <c r="A28" s="17" t="s">
+        <v>131</v>
+      </c>
       <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-    </row>
-    <row r="29" spans="1:250" ht="20.100000000000001" customHeight="1">
-      <c r="A29" s="17"/>
+      <c r="C28" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:250" ht="120" customHeight="1">
+      <c r="A29" s="17" t="s">
+        <v>133</v>
+      </c>
       <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-    </row>
-    <row r="30" spans="1:250" ht="20.100000000000001" customHeight="1">
-      <c r="A30" s="17"/>
+      <c r="C29" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:250" ht="117.75" customHeight="1">
+      <c r="A30" s="17" t="s">
+        <v>137</v>
+      </c>
       <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
+      <c r="C30" s="20" t="s">
+        <v>138</v>
+      </c>
       <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-    </row>
-    <row r="31" spans="1:250" ht="20.100000000000001" customHeight="1">
-      <c r="A31" s="17"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-    </row>
-    <row r="32" spans="1:250" ht="20.100000000000001" customHeight="1">
-      <c r="A32" s="17"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-    </row>
-    <row r="33" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A33" s="17"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-    </row>
-    <row r="34" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A34" s="17"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-    </row>
-    <row r="35" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A35" s="17"/>
+      <c r="E30" s="20" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="31" spans="1:250" ht="205.5" customHeight="1">
+      <c r="A31" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="32" spans="1:250" ht="195.75" customHeight="1">
+      <c r="A32" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="168.75" customHeight="1">
+      <c r="A33" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="170.25" customHeight="1">
+      <c r="A34" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="117" customHeight="1">
+      <c r="A35" s="17" t="s">
+        <v>160</v>
+      </c>
       <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-    </row>
-    <row r="36" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A36" s="17"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-    </row>
-    <row r="37" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A37" s="17"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-    </row>
-    <row r="38" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A38" s="17"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-    </row>
-    <row r="39" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A39" s="17"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-    </row>
-    <row r="40" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A40" s="17"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-    </row>
-    <row r="41" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A41" s="17"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-    </row>
-    <row r="42" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A42" s="17"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-    </row>
-    <row r="43" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A43" s="17"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-    </row>
-    <row r="44" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A44" s="17"/>
+      <c r="C35" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="195" customHeight="1">
+      <c r="A36" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="183.75" customHeight="1">
+      <c r="A37" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="181.5" customHeight="1">
+      <c r="A38" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="D38" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="E38" s="20" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A39" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="B39" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="E39" s="20" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="115.5" customHeight="1">
+      <c r="A40" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="128.25" customHeight="1">
+      <c r="A41" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="128.25" customHeight="1">
+      <c r="A42" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="B42" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="E42" s="20" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="131.25" customHeight="1">
+      <c r="A43" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="D43" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="E43" s="20" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="105" customHeight="1">
+      <c r="A44" s="17" t="s">
+        <v>196</v>
+      </c>
       <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
+      <c r="C44" s="20" t="s">
+        <v>216</v>
+      </c>
       <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-    </row>
-    <row r="45" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A45" s="17"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-    </row>
-    <row r="46" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A46" s="17"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
+      <c r="E44" s="20" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="118.5" customHeight="1">
+      <c r="A45" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="D45" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="E45" s="20" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="143.25" customHeight="1">
+      <c r="A46" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="E46" s="20" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="47" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A47" s="17"/>
@@ -8301,12 +9079,20 @@
       <c r="D52" s="20"/>
       <c r="E52" s="20"/>
     </row>
+    <row r="53" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A53" s="17"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D19" r:id="rId1"/>
+    <hyperlink ref="D27" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Updated IPSL citations file.
</commit_message>
<xml_diff>
--- a/cmip6/citations/cmip6_ipsl_citations.xlsx
+++ b/cmip6/citations/cmip6_ipsl_citations.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="252">
   <si>
     <t>ES-DOC CMIP6 Model Citations</t>
   </si>
@@ -1073,6 +1073,147 @@
   </si>
   <si>
     <t>https://link.springer.com/content/pdf/10.1007/BF00251808.pdf</t>
+  </si>
+  <si>
+    <t>Hourdin2006</t>
+  </si>
+  <si>
+    <t>10.1007/s00382-006-0158-0</t>
+  </si>
+  <si>
+    <t>"@article{
+    author = {Hourdin, F. and {Musat}, I. and {Bony}, S. and {Braconnot}, P. and {Codron}, F. and {Dufresne}, J.-L. and {Fairhead}, L. and {Filiberti}, M.-A. and {Friedlingstein}, P. and {Grandpeix}, J.-Y. and {Krinner}, G. and {Levan}, P. and {Li}, Z.-X. and {Lott}, F.},
+     title = "{The LMDZ4 general circulation model: climate performance and sensitivity to parametrized physics with emphasis on tropical convection}",
+   journal = {Climate Dynamics},
+      year = 2006,
+    volume = 27,
+     pages = {787--813},
+       doi = {10.1007/s00382-006-0158-0}
+}"</t>
+  </si>
+  <si>
+    <t>The LMDZ4 general circulation model: climate performance and sensitivity to parametrized physics with emphasis on tropical convection</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007/s00382-006-0158-0</t>
+  </si>
+  <si>
+    <t>Zhang2017</t>
+  </si>
+  <si>
+    <t>Krinner2005</t>
+  </si>
+  <si>
+    <t>"@article{
+  title={A dynamic global vegetation model for studies of the coupled atmosphere-biosphere system},
+  author={Krinner, Gerhard and Viovy, Nicolas and de Noblet-Ducoudr{\'e}, Nathalie and Og{\'e}e, J{\'e}r{\^o}me and Polcher, Jan and Friedlingstein, Pierre and Ciais, Philippe and Sitch, Stephen and Prentice, I Colin},
+  journal={Global Biogeochemical Cycles},
+  volume={19},
+  number={1},
+  year={2005},
+  publisher={Wiley Online Library}
+}"</t>
+  </si>
+  <si>
+    <t>A dynamic global vegetation model for studies of the coupled atmosphere-biosphere system</t>
+  </si>
+  <si>
+    <t>https://agupubs.onlinelibrary.wiley.com/doi/full/10.1029/2003GB002199</t>
+  </si>
+  <si>
+    <t>10.1029/2003GB002199</t>
+  </si>
+  <si>
+    <t>Ducoudre1993</t>
+  </si>
+  <si>
+    <t>https://journals.ametsoc.org/doi/pdf/10.1175/1520-0442(1993)006%3C0248:SANSOP%3E2.0.CO%3B2</t>
+  </si>
+  <si>
+    <t>deRosnay1998</t>
+  </si>
+  <si>
+    <t>https://hal.archives-ouvertes.fr/file/index/docid/330830/filename/hess-2-239-1998.pdf</t>
+  </si>
+  <si>
+    <t>Modelling root water uptake in a complex land surface scheme coupled to a GCM</t>
+  </si>
+  <si>
+    <t>"@article{
+  title={Modelling root water uptake in a complex land surface scheme coupled to a {GCM}},
+  author={De Rosnay, Patricia and Polcher, Jan},
+  journal={Hydrology and Earth System Sciences Discussions},
+  volume={2},
+  number={2/3},
+  pages={239--255},
+  year={1998}
+}"</t>
+  </si>
+  <si>
+    <t>dOrgeval2008</t>
+  </si>
+  <si>
+    <t>deRosnay2003</t>
+  </si>
+  <si>
+    <t>Farquhar1980</t>
+  </si>
+  <si>
+    <t>Collatz1992</t>
+  </si>
+  <si>
+    <t>Ball1987</t>
+  </si>
+  <si>
+    <t>"@incollection{
+  title={A model predicting stomatal conductance and its contribution to the control of photosynthesis under different environmental conditions},
+  author={Ball, J Timothy and Woodrow, Ian E and Berry, Joseph A},
+  booktitle={Progress in photosynthesis research},
+  pages={221--224},
+  year={1987},
+  publisher={Springer}
+}"</t>
+  </si>
+  <si>
+    <t>A model predicting stomatal conductance and its contribution to the control of photosynthesis under different environmental conditions</t>
+  </si>
+  <si>
+    <t>Zhang2016</t>
+  </si>
+  <si>
+    <t>deRosnay2000</t>
+  </si>
+  <si>
+    <t>"@article{
+  title={Sensitivity of surface fluxes to the number of layers in the soil model used in {GCM}s},
+  author={De Rosnay, P and Bruen, M and Polcher, J},
+  journal={Geophysical research letters},
+  volume={27},
+  number={20},
+  pages={3329--3332},
+  year={2000},
+  publisher={Wiley Online Library}
+}"</t>
+  </si>
+  <si>
+    <t>10.1029/2000GL011574</t>
+  </si>
+  <si>
+    <t>https://agupubs.onlinelibrary.wiley.com/doi/pdf/10.1029/2000GL011574</t>
+  </si>
+  <si>
+    <t>Sensitivity of surface fluxes to the number of layers in the soil model used in GCMs</t>
+  </si>
+  <si>
+    <t>"@article{
+  title={{SECHIBA}, a new set of parameterizations of the hydrologic exchanges at the land-atmosphere interface within the {LMD} atmospheric general circulation model},
+  author={Ducoudr{\'e}, Nathale I and Laval, Katia and Perrier, Alain},
+  journal={Journal of Climate},
+  volume={6},
+  number={2},
+  pages={248--273},
+  year={1993}
+}"</t>
   </si>
 </sst>
 </file>
@@ -3369,10 +3510,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IP53"/>
+  <dimension ref="A1:IP106"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91:XFD106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -9037,54 +9178,487 @@
         <v>202</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A47" s="17"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
+    <row r="47" spans="1:5" ht="154.5" customHeight="1">
+      <c r="A47" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="E47" s="20" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="48" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A48" s="17"/>
+      <c r="A48" s="17" t="s">
+        <v>226</v>
+      </c>
       <c r="B48" s="20"/>
       <c r="C48" s="20"/>
       <c r="D48" s="20"/>
       <c r="E48" s="20"/>
     </row>
-    <row r="49" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A49" s="17"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
-    </row>
-    <row r="50" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A50" s="17"/>
+    <row r="49" spans="1:5" ht="153.75" customHeight="1">
+      <c r="A49" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="B49" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="D49" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="E49" s="20" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="131.25" customHeight="1">
+      <c r="A50" s="17" t="s">
+        <v>232</v>
+      </c>
       <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
+      <c r="C50" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="D50" s="20" t="s">
+        <v>233</v>
+      </c>
       <c r="E50" s="20"/>
     </row>
-    <row r="51" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A51" s="17"/>
+    <row r="51" spans="1:5" ht="118.5" customHeight="1">
+      <c r="A51" s="17" t="s">
+        <v>234</v>
+      </c>
       <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
+      <c r="C51" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="D51" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="E51" s="20" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="52" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A52" s="17"/>
+      <c r="A52" s="17" t="s">
+        <v>238</v>
+      </c>
       <c r="B52" s="20"/>
       <c r="C52" s="20"/>
       <c r="D52" s="20"/>
       <c r="E52" s="20"/>
     </row>
     <row r="53" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A53" s="17"/>
+      <c r="A53" s="17" t="s">
+        <v>239</v>
+      </c>
       <c r="B53" s="20"/>
       <c r="C53" s="20"/>
       <c r="D53" s="20"/>
       <c r="E53" s="20"/>
+    </row>
+    <row r="54" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A54" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="B54" s="20"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20"/>
+    </row>
+    <row r="55" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A55" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="B55" s="20"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="20"/>
+    </row>
+    <row r="56" spans="1:5" ht="117.75" customHeight="1">
+      <c r="A56" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="B56" s="20"/>
+      <c r="C56" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="D56" s="20"/>
+      <c r="E56" s="20" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A57" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="B57" s="20"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="20"/>
+    </row>
+    <row r="58" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A58" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="B58" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="C58" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="D58" s="20" t="s">
+        <v>249</v>
+      </c>
+      <c r="E58" s="20" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A59" s="17"/>
+      <c r="B59" s="20"/>
+      <c r="C59" s="20"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="20"/>
+    </row>
+    <row r="60" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A60" s="17"/>
+      <c r="B60" s="20"/>
+      <c r="C60" s="20"/>
+      <c r="D60" s="20"/>
+      <c r="E60" s="20"/>
+    </row>
+    <row r="61" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A61" s="17"/>
+      <c r="B61" s="20"/>
+      <c r="C61" s="20"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="20"/>
+    </row>
+    <row r="62" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A62" s="17"/>
+      <c r="B62" s="20"/>
+      <c r="C62" s="20"/>
+      <c r="D62" s="20"/>
+      <c r="E62" s="20"/>
+    </row>
+    <row r="63" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A63" s="17"/>
+      <c r="B63" s="20"/>
+      <c r="C63" s="20"/>
+      <c r="D63" s="20"/>
+      <c r="E63" s="20"/>
+    </row>
+    <row r="64" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A64" s="17"/>
+      <c r="B64" s="20"/>
+      <c r="C64" s="20"/>
+      <c r="D64" s="20"/>
+      <c r="E64" s="20"/>
+    </row>
+    <row r="65" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A65" s="17"/>
+      <c r="B65" s="20"/>
+      <c r="C65" s="20"/>
+      <c r="D65" s="20"/>
+      <c r="E65" s="20"/>
+    </row>
+    <row r="66" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A66" s="17"/>
+      <c r="B66" s="20"/>
+      <c r="C66" s="20"/>
+      <c r="D66" s="20"/>
+      <c r="E66" s="20"/>
+    </row>
+    <row r="67" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A67" s="17"/>
+      <c r="B67" s="20"/>
+      <c r="C67" s="20"/>
+      <c r="D67" s="20"/>
+      <c r="E67" s="20"/>
+    </row>
+    <row r="68" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A68" s="17"/>
+      <c r="B68" s="20"/>
+      <c r="C68" s="20"/>
+      <c r="D68" s="20"/>
+      <c r="E68" s="20"/>
+    </row>
+    <row r="69" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A69" s="17"/>
+      <c r="B69" s="20"/>
+      <c r="C69" s="20"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="20"/>
+    </row>
+    <row r="70" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A70" s="17"/>
+      <c r="B70" s="20"/>
+      <c r="C70" s="20"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="20"/>
+    </row>
+    <row r="71" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A71" s="17"/>
+      <c r="B71" s="20"/>
+      <c r="C71" s="20"/>
+      <c r="D71" s="20"/>
+      <c r="E71" s="20"/>
+    </row>
+    <row r="72" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A72" s="17"/>
+      <c r="B72" s="20"/>
+      <c r="C72" s="20"/>
+      <c r="D72" s="20"/>
+      <c r="E72" s="20"/>
+    </row>
+    <row r="73" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A73" s="17"/>
+      <c r="B73" s="20"/>
+      <c r="C73" s="20"/>
+      <c r="D73" s="20"/>
+      <c r="E73" s="20"/>
+    </row>
+    <row r="74" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A74" s="17"/>
+      <c r="B74" s="20"/>
+      <c r="C74" s="20"/>
+      <c r="D74" s="20"/>
+      <c r="E74" s="20"/>
+    </row>
+    <row r="75" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A75" s="17"/>
+      <c r="B75" s="20"/>
+      <c r="C75" s="20"/>
+      <c r="D75" s="20"/>
+      <c r="E75" s="20"/>
+    </row>
+    <row r="76" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A76" s="17"/>
+      <c r="B76" s="20"/>
+      <c r="C76" s="20"/>
+      <c r="D76" s="20"/>
+      <c r="E76" s="20"/>
+    </row>
+    <row r="77" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A77" s="17"/>
+      <c r="B77" s="20"/>
+      <c r="C77" s="20"/>
+      <c r="D77" s="20"/>
+      <c r="E77" s="20"/>
+    </row>
+    <row r="78" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A78" s="17"/>
+      <c r="B78" s="20"/>
+      <c r="C78" s="20"/>
+      <c r="D78" s="20"/>
+      <c r="E78" s="20"/>
+    </row>
+    <row r="79" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A79" s="17"/>
+      <c r="B79" s="20"/>
+      <c r="C79" s="20"/>
+      <c r="D79" s="20"/>
+      <c r="E79" s="20"/>
+    </row>
+    <row r="80" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A80" s="17"/>
+      <c r="B80" s="20"/>
+      <c r="C80" s="20"/>
+      <c r="D80" s="20"/>
+      <c r="E80" s="20"/>
+    </row>
+    <row r="81" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A81" s="17"/>
+      <c r="B81" s="20"/>
+      <c r="C81" s="20"/>
+      <c r="D81" s="20"/>
+      <c r="E81" s="20"/>
+    </row>
+    <row r="82" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A82" s="17"/>
+      <c r="B82" s="20"/>
+      <c r="C82" s="20"/>
+      <c r="D82" s="20"/>
+      <c r="E82" s="20"/>
+    </row>
+    <row r="83" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A83" s="17"/>
+      <c r="B83" s="20"/>
+      <c r="C83" s="20"/>
+      <c r="D83" s="20"/>
+      <c r="E83" s="20"/>
+    </row>
+    <row r="84" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A84" s="17"/>
+      <c r="B84" s="20"/>
+      <c r="C84" s="20"/>
+      <c r="D84" s="20"/>
+      <c r="E84" s="20"/>
+    </row>
+    <row r="85" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A85" s="17"/>
+      <c r="B85" s="20"/>
+      <c r="C85" s="20"/>
+      <c r="D85" s="20"/>
+      <c r="E85" s="20"/>
+    </row>
+    <row r="86" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A86" s="17"/>
+      <c r="B86" s="20"/>
+      <c r="C86" s="20"/>
+      <c r="D86" s="20"/>
+      <c r="E86" s="20"/>
+    </row>
+    <row r="87" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A87" s="17"/>
+      <c r="B87" s="20"/>
+      <c r="C87" s="20"/>
+      <c r="D87" s="20"/>
+      <c r="E87" s="20"/>
+    </row>
+    <row r="88" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A88" s="17"/>
+      <c r="B88" s="20"/>
+      <c r="C88" s="20"/>
+      <c r="D88" s="20"/>
+      <c r="E88" s="20"/>
+    </row>
+    <row r="89" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A89" s="17"/>
+      <c r="B89" s="20"/>
+      <c r="C89" s="20"/>
+      <c r="D89" s="20"/>
+      <c r="E89" s="20"/>
+    </row>
+    <row r="90" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A90" s="17"/>
+      <c r="B90" s="20"/>
+      <c r="C90" s="20"/>
+      <c r="D90" s="20"/>
+      <c r="E90" s="20"/>
+    </row>
+    <row r="91" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A91" s="17"/>
+      <c r="B91" s="20"/>
+      <c r="C91" s="20"/>
+      <c r="D91" s="20"/>
+      <c r="E91" s="20"/>
+    </row>
+    <row r="92" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A92" s="17"/>
+      <c r="B92" s="20"/>
+      <c r="C92" s="20"/>
+      <c r="D92" s="20"/>
+      <c r="E92" s="20"/>
+    </row>
+    <row r="93" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A93" s="17"/>
+      <c r="B93" s="20"/>
+      <c r="C93" s="20"/>
+      <c r="D93" s="20"/>
+      <c r="E93" s="20"/>
+    </row>
+    <row r="94" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A94" s="17"/>
+      <c r="B94" s="20"/>
+      <c r="C94" s="20"/>
+      <c r="D94" s="20"/>
+      <c r="E94" s="20"/>
+    </row>
+    <row r="95" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A95" s="17"/>
+      <c r="B95" s="20"/>
+      <c r="C95" s="20"/>
+      <c r="D95" s="20"/>
+      <c r="E95" s="20"/>
+    </row>
+    <row r="96" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A96" s="17"/>
+      <c r="B96" s="20"/>
+      <c r="C96" s="20"/>
+      <c r="D96" s="20"/>
+      <c r="E96" s="20"/>
+    </row>
+    <row r="97" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A97" s="17"/>
+      <c r="B97" s="20"/>
+      <c r="C97" s="20"/>
+      <c r="D97" s="20"/>
+      <c r="E97" s="20"/>
+    </row>
+    <row r="98" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A98" s="17"/>
+      <c r="B98" s="20"/>
+      <c r="C98" s="20"/>
+      <c r="D98" s="20"/>
+      <c r="E98" s="20"/>
+    </row>
+    <row r="99" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A99" s="17"/>
+      <c r="B99" s="20"/>
+      <c r="C99" s="20"/>
+      <c r="D99" s="20"/>
+      <c r="E99" s="20"/>
+    </row>
+    <row r="100" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A100" s="17"/>
+      <c r="B100" s="20"/>
+      <c r="C100" s="20"/>
+      <c r="D100" s="20"/>
+      <c r="E100" s="20"/>
+    </row>
+    <row r="101" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A101" s="17"/>
+      <c r="B101" s="20"/>
+      <c r="C101" s="20"/>
+      <c r="D101" s="20"/>
+      <c r="E101" s="20"/>
+    </row>
+    <row r="102" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A102" s="17"/>
+      <c r="B102" s="20"/>
+      <c r="C102" s="20"/>
+      <c r="D102" s="20"/>
+      <c r="E102" s="20"/>
+    </row>
+    <row r="103" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A103" s="17"/>
+      <c r="B103" s="20"/>
+      <c r="C103" s="20"/>
+      <c r="D103" s="20"/>
+      <c r="E103" s="20"/>
+    </row>
+    <row r="104" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A104" s="17"/>
+      <c r="B104" s="20"/>
+      <c r="C104" s="20"/>
+      <c r="D104" s="20"/>
+      <c r="E104" s="20"/>
+    </row>
+    <row r="105" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A105" s="17"/>
+      <c r="B105" s="20"/>
+      <c r="C105" s="20"/>
+      <c r="D105" s="20"/>
+      <c r="E105" s="20"/>
+    </row>
+    <row r="106" spans="1:5" ht="130.5" customHeight="1">
+      <c r="A106" s="17"/>
+      <c r="B106" s="20"/>
+      <c r="C106" s="20"/>
+      <c r="D106" s="20"/>
+      <c r="E106" s="20"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>